<commit_message>
add config brain tumor
</commit_message>
<xml_diff>
--- a/w6_7/experiments.xlsx
+++ b/w6_7/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vinbrain-internship\w6_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A731E-FF72-473A-9BE8-D4BE2241530D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA39C5CE-E32A-4B27-830D-0892555591BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="2100" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0;[Red]#,##0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,7 +169,15 @@
       <family val="3"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,8 +185,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,14 +250,15 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,22 +557,22 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
@@ -717,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C089812-934E-4504-8E4A-D88B7C9025AF}">
-  <dimension ref="A5:G16"/>
+  <dimension ref="A5:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +740,10 @@
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.140625" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -747,21 +757,27 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
         <v>0.80459999999999998</v>
       </c>
       <c r="C6" s="8">
         <v>76004833</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="14">
         <v>0.82669999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>0.81389999999999996</v>
+      </c>
+      <c r="F6">
+        <v>0.81320000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -775,7 +791,7 @@
         <v>0.79759999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -785,12 +801,12 @@
       <c r="C8" s="8">
         <v>101529449</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>0.81640000000000001</v>
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -804,7 +820,7 @@
         <v>0.81579999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -817,11 +833,8 @@
       <c r="D10" s="10">
         <v>0.80800000000000005</v>
       </c>
-      <c r="F10" s="13">
-        <v>11181642</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -835,7 +848,7 @@
         <v>0.81610000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -848,23 +861,43 @@
       <c r="D12">
         <v>0.81420000000000003</v>
       </c>
-      <c r="F12" s="13">
+      <c r="H12" s="12">
+        <v>11181642</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H14" s="12">
         <v>62006</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="F14" s="13">
+    <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H16" s="12">
         <v>134301514</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="G15" s="13">
+    <row r="17" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I17" s="12">
         <v>117520202</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="F16" s="13">
+    <row r="18" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H18" s="12">
         <v>21289802</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H20" s="12">
+        <v>23528522</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H21" s="12">
+        <v>25567042</v>
+      </c>
+    </row>
+    <row r="24" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="H24" s="12">
+        <v>6964106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify show batch img
</commit_message>
<xml_diff>
--- a/w6_7/experiments.xlsx
+++ b/w6_7/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vinbrain-internship\w6_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA39C5CE-E32A-4B27-830D-0892555591BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27079104-FC6A-44F9-9951-DC92A3DB2CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -254,11 +254,11 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,22 +557,22 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="60.75" x14ac:dyDescent="0.3">
@@ -727,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C089812-934E-4504-8E4A-D88B7C9025AF}">
-  <dimension ref="A5:I24"/>
+  <dimension ref="A5:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,11 +739,11 @@
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -757,27 +757,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>0.80459999999999998</v>
       </c>
       <c r="C6" s="8">
         <v>76004833</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>0.82669999999999999</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="14">
         <v>0.81389999999999996</v>
       </c>
       <c r="F6">
+        <v>0.81630000000000003</v>
+      </c>
+      <c r="G6">
         <v>0.81320000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -791,7 +794,7 @@
         <v>0.79759999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -805,8 +808,9 @@
         <v>0.81640000000000001</v>
       </c>
       <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -820,7 +824,7 @@
         <v>0.81579999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -834,7 +838,7 @@
         <v>0.80800000000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -848,7 +852,7 @@
         <v>0.81610000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -861,42 +865,42 @@
       <c r="D12">
         <v>0.81420000000000003</v>
       </c>
-      <c r="H12" s="12">
+      <c r="I12" s="12">
         <v>11181642</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="H14" s="12">
+    <row r="14" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I14" s="12">
         <v>62006</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="H16" s="12">
+    <row r="16" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I16" s="12">
         <v>134301514</v>
       </c>
     </row>
-    <row r="17" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="I17" s="12">
+    <row r="17" spans="9:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="J17" s="12">
         <v>117520202</v>
       </c>
     </row>
-    <row r="18" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="H18" s="12">
+    <row r="18" spans="9:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I18" s="12">
         <v>21289802</v>
       </c>
     </row>
-    <row r="20" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="H20" s="12">
+    <row r="20" spans="9:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I20" s="12">
         <v>23528522</v>
       </c>
     </row>
-    <row r="21" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="H21" s="12">
+    <row r="21" spans="9:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I21" s="12">
         <v>25567042</v>
       </c>
     </row>
-    <row r="24" spans="8:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="H24" s="12">
+    <row r="24" spans="9:10" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I24" s="12">
         <v>6964106</v>
       </c>
     </row>

</xml_diff>